<commit_message>
added url to cla
</commit_message>
<xml_diff>
--- a/storage/importer/climbing-rock-areas/EUMA_CLIMBING_ROCK_AREAS_IMPORT_FILE_EXAMPLE.xlsx
+++ b/storage/importer/climbing-rock-areas/EUMA_CLIMBING_ROCK_AREAS_IMPORT_FILE_EXAMPLE.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7miXgFE9fPvKVwdEjyrcy/3Gf6zd4A=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mj7GyrOAQU+E3ABY4vYCdRTVs7wvg=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="121">
   <si>
     <t>id</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>lng</t>
+  </si>
+  <si>
+    <t>url</t>
   </si>
   <si>
     <t>local_rules_url</t>
@@ -382,7 +385,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -405,6 +408,11 @@
       <name val="Arial"/>
     </font>
     <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -413,6 +421,11 @@
       <u/>
       <sz val="10.0"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -430,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -449,7 +462,16 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -673,11 +695,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="22.38"/>
+    <col customWidth="1" min="1" max="1" width="4.88"/>
+    <col customWidth="1" min="2" max="2" width="22.38"/>
     <col customWidth="1" min="3" max="6" width="11.5"/>
-    <col customWidth="1" min="7" max="7" width="35.88"/>
-    <col customWidth="1" min="8" max="17" width="11.5"/>
-    <col customWidth="1" min="18" max="23" width="8.63"/>
+    <col customWidth="1" min="7" max="8" width="35.88"/>
+    <col customWidth="1" min="9" max="18" width="11.5"/>
+    <col customWidth="1" min="19" max="24" width="8.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -708,10 +731,10 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -732,21 +755,24 @@
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4"/>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="T1" s="4"/>
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
       <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="5">
         <v>1.0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -756,24 +782,25 @@
       <c r="F2" s="6">
         <v>15.8882528</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="H2" s="8"/>
+      <c r="N2" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="6">
+      <c r="P2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="6">
         <v>1468.0</v>
       </c>
-      <c r="R2" s="7" t="s">
-        <v>22</v>
+      <c r="S2" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
@@ -781,7 +808,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -791,27 +818,28 @@
       <c r="F3" s="6">
         <v>14.1310358047485</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="5" t="s">
+      <c r="G3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N3" s="6" t="s">
+      <c r="H3" s="11"/>
+      <c r="K3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="6">
+      <c r="N3" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="6">
         <v>1305.0</v>
       </c>
-      <c r="R3" s="7" t="s">
-        <v>22</v>
+      <c r="S3" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
@@ -819,7 +847,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -830,26 +858,27 @@
         <v>15.1824644</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N4" s="6" t="s">
+      <c r="H4" s="6"/>
+      <c r="K4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="6">
+      <c r="N4" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="6">
         <v>3460.0</v>
       </c>
-      <c r="R4" s="7" t="s">
-        <v>22</v>
+      <c r="S4" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
@@ -857,7 +886,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -868,26 +897,27 @@
         <v>15.1658125</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M5" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="K5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="6">
+      <c r="N5" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="6">
         <v>718.0</v>
       </c>
-      <c r="R5" s="7" t="s">
-        <v>22</v>
+      <c r="S5" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
@@ -895,7 +925,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -906,26 +936,27 @@
         <v>15.1755719</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M6" s="6">
+        <v>35</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="K6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" s="6">
         <v>2.0</v>
       </c>
-      <c r="N6" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="6">
+      <c r="O6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="6">
         <v>2422.0</v>
       </c>
-      <c r="R6" s="7" t="s">
-        <v>22</v>
+      <c r="S6" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
@@ -933,7 +964,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -944,26 +975,27 @@
         <v>15.2830123901367</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M7" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="K7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="6">
+      <c r="N7" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="6">
         <v>2978.0</v>
       </c>
-      <c r="R7" s="7" t="s">
-        <v>22</v>
+      <c r="S7" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
@@ -971,7 +1003,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -982,26 +1014,27 @@
         <v>15.1475436</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M8" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="K8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="6">
+      <c r="N8" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="6">
         <v>4824.0</v>
       </c>
-      <c r="R8" s="7" t="s">
-        <v>22</v>
+      <c r="S8" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
@@ -1009,7 +1042,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -1020,26 +1053,27 @@
         <v>15.0459508</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M9" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="K9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="6">
+      <c r="N9" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="6">
         <v>2534.0</v>
       </c>
-      <c r="R9" s="7" t="s">
-        <v>22</v>
+      <c r="S9" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
@@ -1047,7 +1081,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -1058,26 +1092,27 @@
         <v>15.1570129394531</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J10" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="M10" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="O10" s="5" t="s">
+      <c r="H10" s="6"/>
+      <c r="K10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="N10" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="6">
+      <c r="P10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="6">
         <v>3168.0</v>
       </c>
-      <c r="R10" s="7" t="s">
-        <v>22</v>
+      <c r="S10" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1">
@@ -1085,7 +1120,7 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -1096,26 +1131,27 @@
         <v>14.4866169</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M11" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N11" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="O11" s="7" t="s">
+      <c r="H11" s="6"/>
+      <c r="K11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N11" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O11" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="6">
+      <c r="P11" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="6">
         <v>541.0</v>
       </c>
-      <c r="R11" s="7" t="s">
-        <v>22</v>
+      <c r="S11" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
@@ -1123,7 +1159,7 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -1134,23 +1170,24 @@
         <v>16.2453460693359</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="M12" s="6">
+        <v>50</v>
+      </c>
+      <c r="H12" s="6"/>
+      <c r="N12" s="6">
         <v>1.0</v>
       </c>
-      <c r="N12" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="O12" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="6">
+      <c r="O12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="6">
         <v>504.0</v>
       </c>
-      <c r="R12" s="7" t="s">
-        <v>22</v>
+      <c r="S12" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
@@ -1158,7 +1195,7 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -1169,23 +1206,24 @@
         <v>16.709975</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="M13" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="O13" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="6">
+        <v>52</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="N13" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="6">
         <v>1343.0</v>
       </c>
-      <c r="R13" s="7" t="s">
-        <v>22</v>
+      <c r="S13" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
@@ -1193,7 +1231,7 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -1204,26 +1242,27 @@
         <v>14.5711883</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M14" s="6">
+        <v>54</v>
+      </c>
+      <c r="H14" s="6"/>
+      <c r="K14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N14" s="6">
         <v>2.0</v>
       </c>
-      <c r="N14" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="O14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="6">
+      <c r="O14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="6">
         <v>9416.0</v>
       </c>
-      <c r="R14" s="7" t="s">
-        <v>22</v>
+      <c r="S14" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1">
@@ -1231,7 +1270,7 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -1242,26 +1281,27 @@
         <v>14.0501861</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M15" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N15" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="K15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O15" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="6">
+      <c r="N15" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P15" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="6">
         <v>3665.0</v>
       </c>
-      <c r="R15" s="7" t="s">
-        <v>22</v>
+      <c r="S15" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1">
@@ -1269,7 +1309,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -1280,26 +1320,27 @@
         <v>14.017005</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M16" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N16" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="K16" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="6">
+      <c r="N16" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="6">
         <v>1580.0</v>
       </c>
-      <c r="R16" s="7" t="s">
-        <v>22</v>
+      <c r="S16" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1">
@@ -1307,7 +1348,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -1318,26 +1359,27 @@
         <v>14.0335692</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M17" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="K17" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O17" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="6">
+      <c r="N17" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="6">
         <v>2892.0</v>
       </c>
-      <c r="R17" s="7" t="s">
-        <v>22</v>
+      <c r="S17" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="18" ht="12.75" customHeight="1">
@@ -1345,7 +1387,7 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -1356,26 +1398,27 @@
         <v>14.1030922</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M18" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N18" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="K18" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O18" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="6">
+      <c r="N18" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P18" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="6">
         <v>729.0</v>
       </c>
-      <c r="R18" s="7" t="s">
-        <v>22</v>
+      <c r="S18" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1">
@@ -1383,7 +1426,7 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -1394,26 +1437,27 @@
         <v>14.1738167</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M19" s="6">
+        <v>64</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="K19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N19" s="6">
         <v>2.0</v>
       </c>
-      <c r="N19" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="O19" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="6">
+      <c r="O19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P19" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="6">
         <v>914.0</v>
       </c>
-      <c r="R19" s="7" t="s">
-        <v>22</v>
+      <c r="S19" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="20" ht="12.75" customHeight="1">
@@ -1421,7 +1465,7 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -1432,26 +1476,27 @@
         <v>14.2333831</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="J20" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N20" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="O20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="6">
+      <c r="H20" s="6"/>
+      <c r="K20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N20" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="6">
         <v>4249.0</v>
       </c>
-      <c r="R20" s="7" t="s">
-        <v>22</v>
+      <c r="S20" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="21" ht="12.75" customHeight="1">
@@ -1459,7 +1504,7 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -1470,26 +1515,27 @@
         <v>14.2177267</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="M21" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N21" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="O21" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="6">
+        <v>69</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="K21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N21" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="6">
         <v>2314.0</v>
       </c>
-      <c r="R21" s="7" t="s">
-        <v>22</v>
+      <c r="S21" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="22" ht="12.75" customHeight="1">
@@ -1497,7 +1543,7 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -1508,26 +1554,27 @@
         <v>14.3842733</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M22" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N22" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" s="6"/>
+      <c r="K22" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O22" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="6">
+      <c r="N22" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P22" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="6">
         <v>1070.0</v>
       </c>
-      <c r="R22" s="7" t="s">
-        <v>22</v>
+      <c r="S22" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="23" ht="12.75" customHeight="1">
@@ -1535,7 +1582,7 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -1546,26 +1593,27 @@
         <v>14.2924347</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M23" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N23" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H23" s="6"/>
+      <c r="K23" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O23" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="6">
+      <c r="N23" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O23" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="6">
         <v>2915.0</v>
       </c>
-      <c r="R23" s="7" t="s">
-        <v>22</v>
+      <c r="S23" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="24" ht="12.75" customHeight="1">
@@ -1573,7 +1621,7 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -1584,20 +1632,21 @@
         <v>14.5613017</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="M24" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="O24" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="6">
+        <v>75</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="N24" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="P24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="6">
         <v>746.0</v>
       </c>
-      <c r="R24" s="7" t="s">
-        <v>22</v>
+      <c r="S24" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="25" ht="12.75" customHeight="1">
@@ -1605,7 +1654,7 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -1616,23 +1665,24 @@
         <v>14.5815125</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="J25" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="M25" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="O25" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="6">
+      <c r="H25" s="6"/>
+      <c r="K25" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="N25" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="P25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="6">
         <v>820.0</v>
       </c>
-      <c r="R25" s="7" t="s">
-        <v>22</v>
+      <c r="S25" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="26" ht="12.75" customHeight="1">
@@ -1640,7 +1690,7 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -1651,26 +1701,27 @@
         <v>14.8259261</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M26" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N26" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="K26" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O26" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="P26" s="7"/>
-      <c r="Q26" s="6">
+      <c r="N26" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P26" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="6">
         <v>719.0</v>
       </c>
-      <c r="R26" s="7" t="s">
-        <v>22</v>
+      <c r="S26" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1">
@@ -1678,7 +1729,7 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -1689,23 +1740,24 @@
         <v>17.3194722</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="M27" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N27" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="O27" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="P27" s="7"/>
-      <c r="Q27" s="6">
+        <v>82</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="N27" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P27" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="6">
         <v>640.0</v>
       </c>
-      <c r="R27" s="7" t="s">
-        <v>22</v>
+      <c r="S27" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="28" ht="12.75" customHeight="1">
@@ -1713,7 +1765,7 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -1724,20 +1776,21 @@
         <v>14.3693928</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="M28" s="6">
+        <v>84</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="N28" s="6">
         <v>2.0</v>
       </c>
-      <c r="O28" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="6">
+      <c r="P28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="6">
         <v>861.0</v>
       </c>
-      <c r="R28" s="7" t="s">
-        <v>22</v>
+      <c r="S28" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="29" ht="12.75" customHeight="1">
@@ -1745,7 +1798,7 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -1756,26 +1809,27 @@
         <v>14.2569547</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="J29" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="M29" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N29" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="O29" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="P29" s="7"/>
-      <c r="Q29" s="6">
+      <c r="H29" s="6"/>
+      <c r="K29" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="N29" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="P29" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="6">
         <v>1171.0</v>
       </c>
-      <c r="R29" s="7" t="s">
-        <v>22</v>
+      <c r="S29" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="30" ht="12.75" customHeight="1">
@@ -1783,7 +1837,7 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -1794,20 +1848,21 @@
         <v>17.1242147</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="M30" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="O30" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="P30" s="7"/>
-      <c r="Q30" s="6">
+        <v>89</v>
+      </c>
+      <c r="H30" s="6"/>
+      <c r="N30" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="P30" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="6">
         <v>1655.0</v>
       </c>
-      <c r="R30" s="7" t="s">
-        <v>22</v>
+      <c r="S30" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1">
@@ -1815,7 +1870,7 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -1826,23 +1881,24 @@
         <v>14.2494111</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="M31" s="6">
+        <v>91</v>
+      </c>
+      <c r="H31" s="6"/>
+      <c r="N31" s="6">
         <v>2.0</v>
       </c>
-      <c r="N31" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="O31" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="6">
+      <c r="O31" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="P31" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="6">
         <v>1573.0</v>
       </c>
-      <c r="R31" s="7" t="s">
-        <v>22</v>
+      <c r="S31" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="32" ht="12.75" customHeight="1">
@@ -1850,7 +1906,7 @@
         <v>31.0</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
@@ -1861,20 +1917,21 @@
         <v>13.2221894</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="M32" s="6">
+        <v>94</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="N32" s="6">
         <v>2.0</v>
       </c>
-      <c r="O32" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="6">
+      <c r="P32" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="6">
         <v>4051.0</v>
       </c>
-      <c r="R32" s="7" t="s">
-        <v>22</v>
+      <c r="S32" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="33" ht="12.75" customHeight="1">
@@ -1882,7 +1939,7 @@
         <v>32.0</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
@@ -1893,20 +1950,21 @@
         <v>13.1533436</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="M33" s="6">
+        <v>96</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="N33" s="6">
         <v>2.0</v>
       </c>
-      <c r="O33" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="6">
+      <c r="P33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="6">
         <v>812.0</v>
       </c>
-      <c r="R33" s="7" t="s">
-        <v>22</v>
+      <c r="S33" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="34" ht="12.75" customHeight="1">
@@ -1914,7 +1972,7 @@
         <v>33.0</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -1925,26 +1983,27 @@
         <v>16.114023</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M34" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N34" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H34" s="6"/>
+      <c r="K34" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O34" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P34" s="5"/>
-      <c r="Q34" s="6">
+      <c r="N34" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O34" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="6">
         <v>6099.0</v>
       </c>
-      <c r="R34" s="7" t="s">
-        <v>22</v>
+      <c r="S34" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="35" ht="12.75" customHeight="1">
@@ -1952,7 +2011,7 @@
         <v>34.0</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
@@ -1963,26 +2022,27 @@
         <v>16.2976319</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="J35" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M35" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N35" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H35" s="6"/>
+      <c r="K35" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O35" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P35" s="5"/>
-      <c r="Q35" s="6">
+      <c r="N35" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O35" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="6">
         <v>1341.0</v>
       </c>
-      <c r="R35" s="7" t="s">
-        <v>22</v>
+      <c r="S35" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="36" ht="12.75" customHeight="1">
@@ -1990,7 +2050,7 @@
         <v>35.0</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
@@ -2001,26 +2061,27 @@
         <v>16.1285581</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="J36" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M36" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N36" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="H36" s="6"/>
+      <c r="K36" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O36" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="6">
+      <c r="N36" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O36" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P36" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="6">
         <v>1665.0</v>
       </c>
-      <c r="R36" s="7" t="s">
-        <v>22</v>
+      <c r="S36" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="37" ht="12.75" customHeight="1">
@@ -2028,7 +2089,7 @@
         <v>36.0</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -2039,26 +2100,27 @@
         <v>16.212646</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M37" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N37" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H37" s="6"/>
+      <c r="K37" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O37" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="P37" s="7"/>
-      <c r="Q37" s="6">
+      <c r="N37" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O37" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P37" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q37" s="9"/>
+      <c r="R37" s="6">
         <v>1267.0</v>
       </c>
-      <c r="R37" s="7" t="s">
-        <v>22</v>
+      <c r="S37" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="38" ht="12.75" customHeight="1">
@@ -2066,7 +2128,7 @@
         <v>37.0</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
@@ -2077,26 +2139,27 @@
         <v>16.1323928833008</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="J38" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M38" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N38" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H38" s="6"/>
+      <c r="K38" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O38" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P38" s="5"/>
-      <c r="Q38" s="6">
+      <c r="N38" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O38" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P38" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="6">
         <v>2383.0</v>
       </c>
-      <c r="R38" s="7" t="s">
-        <v>22</v>
+      <c r="S38" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="39" ht="12.75" customHeight="1">
@@ -2104,7 +2167,7 @@
         <v>38.0</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
@@ -2115,26 +2178,27 @@
         <v>13.35886</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="J39" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="M39" s="6">
+      <c r="H39" s="6"/>
+      <c r="K39" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="N39" s="6">
         <v>2.0</v>
       </c>
-      <c r="N39" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="O39" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="P39" s="7"/>
-      <c r="Q39" s="6">
+      <c r="O39" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="P39" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q39" s="9"/>
+      <c r="R39" s="6">
         <v>761.0</v>
       </c>
-      <c r="R39" s="7" t="s">
-        <v>22</v>
+      <c r="S39" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="40" ht="12.75" customHeight="1">
@@ -2142,7 +2206,7 @@
         <v>39.0</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
@@ -2153,26 +2217,27 @@
         <v>13.4465789</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="J40" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="M40" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N40" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="O40" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="P40" s="7"/>
-      <c r="Q40" s="6">
+      <c r="H40" s="6"/>
+      <c r="K40" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="N40" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O40" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="P40" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q40" s="9"/>
+      <c r="R40" s="6">
         <v>3309.0</v>
       </c>
-      <c r="R40" s="7" t="s">
-        <v>22</v>
+      <c r="S40" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="41" ht="12.75" customHeight="1">
@@ -2180,7 +2245,7 @@
         <v>40.0</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
@@ -2191,20 +2256,21 @@
         <v>13.4956564</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="M41" s="6">
+        <v>114</v>
+      </c>
+      <c r="H41" s="6"/>
+      <c r="N41" s="6">
         <v>2.0</v>
       </c>
-      <c r="O41" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="P41" s="7"/>
-      <c r="Q41" s="6">
+      <c r="P41" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q41" s="9"/>
+      <c r="R41" s="6">
         <v>686.0</v>
       </c>
-      <c r="R41" s="7" t="s">
-        <v>22</v>
+      <c r="S41" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="42" ht="12.75" customHeight="1">
@@ -2212,7 +2278,7 @@
         <v>41.0</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
@@ -2223,23 +2289,24 @@
         <v>13.1580303</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="J42" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M42" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="O42" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="P42" s="7"/>
-      <c r="Q42" s="6">
+        <v>116</v>
+      </c>
+      <c r="H42" s="6"/>
+      <c r="K42" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N42" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="P42" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q42" s="9"/>
+      <c r="R42" s="6">
         <v>821.0</v>
       </c>
-      <c r="R42" s="7" t="s">
-        <v>22</v>
+      <c r="S42" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="43" ht="12.75" customHeight="1">
@@ -2247,7 +2314,7 @@
         <v>42.0</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
@@ -2258,20 +2325,21 @@
         <v>13.6613503</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="M43" s="6">
+        <v>118</v>
+      </c>
+      <c r="H43" s="6"/>
+      <c r="N43" s="6">
         <v>2.0</v>
       </c>
-      <c r="O43" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="P43" s="5"/>
-      <c r="Q43" s="6">
+      <c r="P43" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q43" s="5"/>
+      <c r="R43" s="6">
         <v>518.0</v>
       </c>
-      <c r="R43" s="7" t="s">
-        <v>22</v>
+      <c r="S43" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="44" ht="12.75" customHeight="1">
@@ -2279,7 +2347,7 @@
         <v>43.0</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
@@ -2290,31 +2358,33 @@
         <v>13.3472614</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="J44" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="M44" s="6">
-        <v>3.0</v>
-      </c>
-      <c r="N44" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="O44" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="P44" s="7"/>
-      <c r="Q44" s="6">
+        <v>120</v>
+      </c>
+      <c r="H44" s="6"/>
+      <c r="K44" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="N44" s="6">
+        <v>3.0</v>
+      </c>
+      <c r="O44" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="P44" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q44" s="9"/>
+      <c r="R44" s="6">
         <v>1722.0</v>
       </c>
-      <c r="R44" s="7" t="s">
-        <v>22</v>
+      <c r="S44" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="G3"/>
+    <hyperlink r:id="rId1" ref="G2"/>
+    <hyperlink r:id="rId2" ref="G3"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="1.025" footer="0.0" header="0.0" left="0.7875" right="0.7875" top="1.025"/>
@@ -2323,6 +2393,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CStránka &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>